<commit_message>
Added Journal.md from an external Journal app, edited README.md
</commit_message>
<xml_diff>
--- a/LearningRoadmapTracker.xlsx
+++ b/LearningRoadmapTracker.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D671391D-2E15-4F7C-9036-586733FD0D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061A6685-7F00-456C-9FC1-9A9B0F9CF2E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Roadmap" sheetId="1" r:id="rId1"/>
@@ -511,7 +511,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Edited Journal.md and Progress Tracker
</commit_message>
<xml_diff>
--- a/LearningRoadmapTracker.xlsx
+++ b/LearningRoadmapTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061A6685-7F00-456C-9FC1-9A9B0F9CF2E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EAE170A-FCA5-41B1-88F9-CF58F6DBBAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -511,7 +511,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Changes made in LearningRoadmapTracker.xlsx, Day 8.md Added Day 9.md, text_stats.py, text_summary.py, text.txt
</commit_message>
<xml_diff>
--- a/LearningRoadmapTracker.xlsx
+++ b/LearningRoadmapTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD8FF35-3E3C-40CC-8D5B-B42CFF8E833B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4AC35A4-8CF8-41C1-AB0A-F705C4F68A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="18195" windowHeight="7576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Roadmap" sheetId="1" r:id="rId1"/>
@@ -511,10 +511,10 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="66" customWidth="1"/>
@@ -525,7 +525,7 @@
     <col min="8" max="8" width="60" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -549,10 +549,10 @@
       </c>
       <c r="H1" s="2">
         <f>IF(COUNTA(A2:A17)=0,0,COUNTIF(E2:E17,"☑")/COUNTA(A2:A17))</f>
-        <v>0.1875</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -570,7 +570,7 @@
       </c>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -588,7 +588,7 @@
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -606,7 +606,7 @@
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -614,17 +614,17 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -632,17 +632,17 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -660,7 +660,7 @@
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -678,7 +678,7 @@
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -696,7 +696,7 @@
       </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -714,7 +714,7 @@
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -732,7 +732,7 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -750,7 +750,7 @@
       </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -768,7 +768,7 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -786,7 +786,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -804,7 +804,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -822,7 +822,7 @@
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Changes made in LearningRoadmapTracker.xlsx, Day 9, 10, 11, 12.md
</commit_message>
<xml_diff>
--- a/LearningRoadmapTracker.xlsx
+++ b/LearningRoadmapTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4AC35A4-8CF8-41C1-AB0A-F705C4F68A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606373A5-84CE-4C31-BDCD-3D7B35180885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="18195" windowHeight="7576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="33">
   <si>
     <t>Phase</t>
   </si>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t>Done</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -510,8 +507,8 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -549,7 +546,7 @@
       </c>
       <c r="H1" s="2">
         <f>IF(COUNTA(A2:A17)=0,0,COUNTIF(E2:E17,"☑")/COUNTA(A2:A17))</f>
-        <v>0.25</v>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
@@ -632,13 +629,13 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="F6" s="4"/>
     </row>

</xml_diff>

<commit_message>
Changes made in LearningRoadmapTracker.xlsx
Added Day 13.md
</commit_message>
<xml_diff>
--- a/LearningRoadmapTracker.xlsx
+++ b/LearningRoadmapTracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606373A5-84CE-4C31-BDCD-3D7B35180885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F034F6E-69AE-414F-9CC3-D4A12D7491D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="18195" windowHeight="7576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Roadmap" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="34">
   <si>
     <t>Phase</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -508,10 +511,10 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="66" customWidth="1"/>
@@ -522,7 +525,7 @@
     <col min="8" max="8" width="60" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -549,7 +552,7 @@
         <v>0.3125</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -567,7 +570,7 @@
       </c>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -585,7 +588,7 @@
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -603,7 +606,7 @@
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -621,7 +624,7 @@
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -639,7 +642,7 @@
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -647,17 +650,17 @@
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -675,7 +678,7 @@
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -693,7 +696,7 @@
       </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -711,7 +714,7 @@
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -729,7 +732,7 @@
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -747,7 +750,7 @@
       </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -765,7 +768,7 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -783,7 +786,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -801,7 +804,7 @@
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -819,7 +822,7 @@
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
- Renamed Day 14 -> Day 14 & 15.md - Updated LearningRoadmapTracker.xlsx
</commit_message>
<xml_diff>
--- a/LearningRoadmapTracker.xlsx
+++ b/LearningRoadmapTracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F034F6E-69AE-414F-9CC3-D4A12D7491D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85FA2EE-FD75-4C7D-84F0-D68AB23F6713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Roadmap" sheetId="1" r:id="rId1"/>
@@ -511,7 +511,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,7 +549,7 @@
       </c>
       <c r="H1" s="2">
         <f>IF(COUNTA(A2:A17)=0,0,COUNTIF(E2:E17,"☑")/COUNTA(A2:A17))</f>
-        <v>0.3125</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -650,13 +650,13 @@
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="F7" s="4"/>
     </row>
@@ -668,10 +668,10 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
- Add notes for Days 19-21 and update Learning Roadmap Tracker
</commit_message>
<xml_diff>
--- a/LearningRoadmapTracker.xlsx
+++ b/LearningRoadmapTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A85FA2EE-FD75-4C7D-84F0-D68AB23F6713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3851E352-AAF2-4AD2-ABD7-7397185FDE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -511,7 +511,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,7 +549,7 @@
       </c>
       <c r="H1" s="2">
         <f>IF(COUNTA(A2:A17)=0,0,COUNTIF(E2:E17,"☑")/COUNTA(A2:A17))</f>
-        <v>0.375</v>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -668,13 +668,13 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="F8" s="4"/>
     </row>
@@ -686,10 +686,10 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
docs(journal): add entry for Day 22 on Nmap and Wireshark
- Document learning activities for Day 22, focusing on network scanning.
- Cover initial studies on Wireshark fundamentals and packet filtering.
- Note resources used, including YouTube tutorials and practice sites.
- Update the learning roadmap tracker to reflect the day's progress.
- Rename the journal file to include the latest day.
</commit_message>
<xml_diff>
--- a/LearningRoadmapTracker.xlsx
+++ b/LearningRoadmapTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3851E352-AAF2-4AD2-ABD7-7397185FDE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88913C4B-C3B8-48F2-BCC3-9ED4FBD702C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -511,7 +511,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,7 +549,7 @@
       </c>
       <c r="H1" s="2">
         <f>IF(COUNTA(A2:A17)=0,0,COUNTIF(E2:E17,"☑")/COUNTA(A2:A17))</f>
-        <v>0.4375</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -686,13 +686,13 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="F9" s="4"/>
     </row>
@@ -704,10 +704,10 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
docs(journal): add entries for Day 23 and Day 24
- Documents learning on Nmap for Day 23, covering various scan types.
- Adds notes for Day 24 on practical hacking with the TryHackMe Vulnversity room.
- Topics covered include reconnaissance, GoBuster, and privilege escalation.
- Consolidates the Day 23 log into a new combined file with Day 24.
- Updates the learning roadmap tracker to reflect recent progress.
</commit_message>
<xml_diff>
--- a/LearningRoadmapTracker.xlsx
+++ b/LearningRoadmapTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88913C4B-C3B8-48F2-BCC3-9ED4FBD702C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9400DB8A-A9C9-4605-9E9F-E980EA24769C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -511,7 +511,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,7 +549,7 @@
       </c>
       <c r="H1" s="2">
         <f>IF(COUNTA(A2:A17)=0,0,COUNTIF(E2:E17,"☑")/COUNTA(A2:A17))</f>
-        <v>0.5</v>
+        <v>0.5625</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -704,13 +704,13 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="F10" s="4"/>
     </row>
@@ -722,10 +722,10 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>10</v>
@@ -859,5 +859,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>